<commit_message>
Migraciones finalizadas de Uber y de Factoraje
</commit_message>
<xml_diff>
--- a/UberClients.xlsx
+++ b/UberClients.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="101">
   <si>
     <t>Nombre</t>
   </si>
@@ -315,13 +315,25 @@
   </si>
   <si>
     <t>MOAJ700302PDA</t>
+  </si>
+  <si>
+    <t>Recuperacion Total sin IVA</t>
+  </si>
+  <si>
+    <t>Intereses</t>
+  </si>
+  <si>
+    <t>% de Intereses</t>
+  </si>
+  <si>
+    <t>Fecha Inicio de Prestamo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,8 +364,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,8 +392,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -381,11 +407,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -401,6 +442,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +743,7 @@
     <col min="6" max="6" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -730,8 +777,9 @@
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -766,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -801,7 +849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -836,7 +884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>25031</v>
       </c>
@@ -871,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -906,7 +954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5556843950</v>
       </c>
@@ -941,7 +989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -976,7 +1024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1011,7 +1059,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1046,7 +1094,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1081,7 +1129,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1116,7 +1164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1151,7 +1199,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1186,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1221,7 +1269,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2059,6 +2107,146 @@
       </c>
       <c r="K39" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>533303.40150344756</v>
+      </c>
+      <c r="B40">
+        <v>376388.77241379436</v>
+      </c>
+      <c r="C40">
+        <v>428756.93001379352</v>
+      </c>
+      <c r="D40">
+        <v>377628.76866207027</v>
+      </c>
+      <c r="E40">
+        <v>428275.90193103498</v>
+      </c>
+      <c r="F40">
+        <v>427236.39273103501</v>
+      </c>
+      <c r="G40">
+        <v>377628.76866207027</v>
+      </c>
+      <c r="H40">
+        <v>427512.25111724186</v>
+      </c>
+      <c r="I40">
+        <v>427236.39031724189</v>
+      </c>
+      <c r="J40">
+        <v>426798.45529655222</v>
+      </c>
+      <c r="K40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>310827.15295172343</v>
+      </c>
+      <c r="B41">
+        <v>126759.14827586332</v>
+      </c>
+      <c r="C41">
+        <v>178927.96920000046</v>
+      </c>
+      <c r="D41">
+        <v>126759.14452413924</v>
+      </c>
+      <c r="E41">
+        <v>178446.94111724192</v>
+      </c>
+      <c r="F41">
+        <v>183467.54053793161</v>
+      </c>
+      <c r="G41">
+        <v>126759.14452413924</v>
+      </c>
+      <c r="H41">
+        <v>183743.39892413846</v>
+      </c>
+      <c r="I41">
+        <v>183467.53812413849</v>
+      </c>
+      <c r="J41">
+        <v>182915.81893793162</v>
+      </c>
+      <c r="K41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.58283362167851105</v>
+      </c>
+      <c r="B42">
+        <v>0.33679999999999999</v>
+      </c>
+      <c r="C42">
+        <v>0.4173</v>
+      </c>
+      <c r="D42">
+        <v>0.3357</v>
+      </c>
+      <c r="E42">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="F42">
+        <v>0.4294</v>
+      </c>
+      <c r="G42">
+        <v>0.3357</v>
+      </c>
+      <c r="H42">
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="I42">
+        <v>0.4294</v>
+      </c>
+      <c r="J42">
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="K42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>42963</v>
+      </c>
+      <c r="B43" s="5">
+        <v>42972</v>
+      </c>
+      <c r="C43" s="7">
+        <v>43007</v>
+      </c>
+      <c r="D43" s="7">
+        <v>43056</v>
+      </c>
+      <c r="E43" s="7">
+        <v>43011</v>
+      </c>
+      <c r="F43" s="8">
+        <v>43082</v>
+      </c>
+      <c r="G43" s="7">
+        <v>43046</v>
+      </c>
+      <c r="H43" s="7">
+        <v>43063</v>
+      </c>
+      <c r="I43" s="7">
+        <v>43067</v>
+      </c>
+      <c r="J43" s="8">
+        <v>43074</v>
+      </c>
+      <c r="K43" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>